<commit_message>
Noticias sobre las elecciones presidenciales.
</commit_message>
<xml_diff>
--- a/EstudioMedios.xlsx
+++ b/EstudioMedios.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Asignación General" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -114,6 +114,60 @@
   </si>
   <si>
     <t>Las recientes encuestas muestran un empate técnico entre Sergio Fajardo e Iván Duque</t>
+  </si>
+  <si>
+    <t>http://www.elcolombiano.com/colombia/politica/derecha-e-izquierda-de-nuevo-las-protagonistas-FI8309447</t>
+  </si>
+  <si>
+    <t>Marzo 6/2018</t>
+  </si>
+  <si>
+    <t>Derecha e izquierda de nuevo las protagonistas</t>
+  </si>
+  <si>
+    <t>Santos dice que fue un "error" que Farc se presentaran a contienda electoral tan rápido</t>
+  </si>
+  <si>
+    <t>Marzo 8/2018</t>
+  </si>
+  <si>
+    <t>http://www.elcolombiano.com/elecciones-2018-colombia/santos-entiende-retiro-de-timochenko-de-la-contienda-electoral-FA8332061</t>
+  </si>
+  <si>
+    <t>Sin candidato presidencial, Farc se conforma con el congreso</t>
+  </si>
+  <si>
+    <t>Marzo 9/2018</t>
+  </si>
+  <si>
+    <t>http://www.elcolombiano.com/colombia/politica/sin-candidato-presidencial-farc-se-conforma-con-el-congreso-AB8333626</t>
+  </si>
+  <si>
+    <t>Los candidatos colombianos que copieron propagandas extrangeras</t>
+  </si>
+  <si>
+    <t>http://www.elcolombiano.com/elecciones-2018-colombia/candidatos-colombianos-que-copiaron-propagandas-extranjeras-FF8337878</t>
+  </si>
+  <si>
+    <t>Por fin habrá tarjetón presidencial.</t>
+  </si>
+  <si>
+    <t>Marzo 10/2018</t>
+  </si>
+  <si>
+    <t>http://www.elcolombiano.com/elecciones-2018-colombia/por-fin-habra-tarjeton-presidencial-XE8341761</t>
+  </si>
+  <si>
+    <t>El Vice, una figura con un poder creciente</t>
+  </si>
+  <si>
+    <t>http://www.elcolombiano.com/elecciones-2018-colombia/el-vice-una-figura-con-un-poder-creciente-CD8342602</t>
+  </si>
+  <si>
+    <t>Estos son los Candidatos Transparentes.</t>
+  </si>
+  <si>
+    <t>http://www.elcolombiano.com/elecciones-2018-colombia/estos-son-los-candidatos-transparentes-BD8342641</t>
   </si>
 </sst>
 </file>
@@ -469,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1503,14 +1557,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" customWidth="1"/>
     <col min="4" max="4" width="112.28515625" customWidth="1"/>
   </cols>
@@ -1544,46 +1598,88 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>

</xml_diff>

<commit_message>
Noticias de la revista Dinero
</commit_message>
<xml_diff>
--- a/EstudioMedios.xlsx
+++ b/EstudioMedios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejo\Documents\BigData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBA1809-9F74-477A-801C-E7F15E1C17FC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DE462A-92F8-4A87-9591-80499BFA8239}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -127,13 +127,103 @@
   </si>
   <si>
     <t>http://www.dinero.com/economia/multimedia/sergio-fajardo-en-al-tablero/256007</t>
+  </si>
+  <si>
+    <t>http://www.dinero.com/inversionistas/articulo/peso-colombiano-se-mantiene-gracias-al-petroleo-y-las-encuestas/256927</t>
+  </si>
+  <si>
+    <t>Las encuesta de intención de voto para las elecciones presidenciales muestran una mayor probabilidad de victoria para candidatos pro mercado.</t>
+  </si>
+  <si>
+    <t>Encuestas y petróleo le ayudan al peso colombiano</t>
+  </si>
+  <si>
+    <t>Iván Duque es el candidato de la coalición del No</t>
+  </si>
+  <si>
+    <t>Este domingo se llevaron a cabo las elecciones para senadores y representantes a la Cámara, a la vez que se realizaron las consultas “Inclusión Social para la Paz” y “Gran Consulta por Colombia” que dejó como ganador al candidato del Centro Democrático.</t>
+  </si>
+  <si>
+    <t>http://www.dinero.com/pais/articulo/ivan-duque-elegido-como-candidato-presidencial/256231</t>
+  </si>
+  <si>
+    <t>Iván Duque: propuestas económicas para la presidencia</t>
+  </si>
+  <si>
+    <t>El candidato presidencial del Centro Democrático, Iván Duque, en 'Al Tablero', hablando sobre sus propuestas económicas de cara a las elecciones de mayo. Usted puede seguir la transmisión en este espacio y realizar sus preguntas a través de la página de Facebook o desde twitter.</t>
+  </si>
+  <si>
+    <t>http://www.dinero.com/pais/multimedia/propuestas-economicas-de-ivan-duque-en-al-tablero/254580</t>
+  </si>
+  <si>
+    <t>El liderazgo de Gustavo Petro tiene pensando a Wall Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El liderazgo de Gustavo Petro en las encuestas ya tiene pensando a Wall Street. “Los inversionistas no han caído en cuenta de que existe la posibilidad de que este candidato gane y cuando lo hagan se va presentar una fuerte liquidación de los bonos y la moneda colombiana”, </t>
+  </si>
+  <si>
+    <t>http://www.dinero.com/empresas/confidencias-on-line/articulo/gustavo-petro-preocupa-a-wall-street/255306#</t>
+  </si>
+  <si>
+    <t>Gustavo Petro es el candidato presidencial de Inclusión Social para la Paz</t>
+  </si>
+  <si>
+    <t>Gustavo Petro se enfrentaba en la consulta “Inclusión Social para la Paz” al exalcalde de Santa Marta, Carlos Caicedo, quien también había presentado su candidatura por firmas.</t>
+  </si>
+  <si>
+    <t>http://www.dinero.com/pais/articulo/gustavo-petro-elegido-como-candidato-presidencial-2018/256232</t>
+  </si>
+  <si>
+    <t>Gustavo Petro sería riesgoso para relaciones con Estados Unidos</t>
+  </si>
+  <si>
+    <t>Uno de los paneles más importantes que desarrollará el foro de la Cámara de Comercio Colombo Americana (AmCham Colombia) el próximo 22 de marzo en El Nogal es la conclusión de un estudio realizado por Control Risk sobre cuál o cuáles candidatos presidenciales presentan riesgos y darían un giro fuerte en la relación con Estados Unidos, basado en sus posiciones históricas</t>
+  </si>
+  <si>
+    <t>http://www.dinero.com/empresas/confidencias-on-line/articulo/amcham-presenta-estudio-de-control-risk-sobre-candidatos/256320#</t>
+  </si>
+  <si>
+    <t>¿Qué candidato presidencial es el rey de las redes sociales?</t>
+  </si>
+  <si>
+    <t>Mientras Germán Vargas Lleras tiene el hashtag que más se utiliza en Twitter y es el que genera mayor conversación, el candidato Gustavo Petro fue el más mencionado por los usuarios de las redes en el últimos mes.</t>
+  </si>
+  <si>
+    <t>http://www.dinero.com/pais/articulo/el-candidato-presidencial-preferido-en-redes-sociales/256219</t>
+  </si>
+  <si>
+    <t>Propuestas sobre impuestos del candidato Germán Vargas Lleras</t>
+  </si>
+  <si>
+    <t>Dinero le hizo preguntas puntuales en materia de impuestos a los candidatos presidenciales que puntean las encuestas. Aquí las respuestas de Germán Vargas LLeras.</t>
+  </si>
+  <si>
+    <t>http://www.dinero.com/edicion-impresa/caratula/articulo/propuestas-sobre-impuestos-de-german-vargas-lleras/256456</t>
+  </si>
+  <si>
+    <t>Propuestas sobre impuestos del candidato Sergio Fajardo</t>
+  </si>
+  <si>
+    <t>Dinero le hizo preguntas puntuales en materia de impuestos a los candidatos presidenciales que puntean las encuestas. Aquí las respuestas de Sergio Fajardo.</t>
+  </si>
+  <si>
+    <t>http://www.dinero.com/edicion-impresa/caratula/articulo/propuestas-sobre-impuestos-de-sergio-fajardo/256461</t>
+  </si>
+  <si>
+    <t>Sergio Fajardo se compromete a no aumentar la edad de pensión si es presidente</t>
+  </si>
+  <si>
+    <t>El candidato presidencial por Alianza Verde, Sergio Farjardo, se comprometió este viernes a no aumentar la edad para pensionarse, según lo han propuesto diferentes analista e instituciones como reforma al sistema.</t>
+  </si>
+  <si>
+    <t>http://www.dinero.com/edicion-impresa/pais/articulo/sergio-fajardo-se-compromete-a-no-aumentar-la-edad-de-pension/255174</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +238,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri "/>
     </font>
   </fonts>
   <fills count="4">
@@ -198,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -226,6 +321,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -514,13 +627,13 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -528,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -536,7 +649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -544,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -552,7 +665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -560,7 +673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -568,7 +681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -576,7 +689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -584,7 +697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -592,7 +705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -609,18 +722,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="3" max="3" width="29.140625" customWidth="1"/>
     <col min="4" max="4" width="77.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -634,103 +747,197 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" ht="150">
+      <c r="A2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="13">
+        <v>43125</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="120">
+      <c r="A3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="13">
+        <v>43140</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="150">
+      <c r="A4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="13">
+        <v>43151</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="75">
+      <c r="A5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B5" s="7">
         <v>43160</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D5" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="120">
+      <c r="A6" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="13">
+        <v>43169</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="150">
+      <c r="A7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="13">
+        <v>43170</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="105">
+      <c r="A8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="13">
+        <v>43170</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="90">
+      <c r="A9" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="13">
+        <v>43174</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="90">
+      <c r="A10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="13">
+        <v>43174</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="210">
+      <c r="A11" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="13">
+        <v>43179</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="85.5">
+      <c r="A12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="13">
+        <v>43187</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
     </row>
   </sheetData>
+  <sortState ref="A2:D12">
+    <sortCondition ref="B1"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{63E0DD6C-732B-432B-BAEA-AF8B1148C840}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{63E0DD6C-732B-432B-BAEA-AF8B1148C840}"/>
+    <hyperlink ref="D12" r:id="rId2" xr:uid="{E18585DB-5C71-4139-A4B5-B348E2209054}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{17DA8C2D-C869-416D-9C1E-714DB389F230}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{44A3A4E3-E92B-40C1-AEF3-6EB4130284FC}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{3B297BC8-D37A-42C7-B5E8-6066658657FD}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{F49E5180-BCA4-4418-806D-51AB3D73C171}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{D9A14D56-1C4C-47ED-8028-97D20B996B0E}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{5561941F-5F29-4CE4-B617-9E58DA9E6CBA}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{4EF24BDC-D7C3-4D56-8B81-9DE3EC4D03D0}"/>
+    <hyperlink ref="D10" r:id="rId10" xr:uid="{EE1C8E74-1F51-4684-AE14-92565BF88E09}"/>
+    <hyperlink ref="D3" r:id="rId11" xr:uid="{C1EB246C-8444-4D45-92AF-A5D9A3B88871}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -742,13 +949,13 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="3" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -762,85 +969,85 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -859,14 +1066,14 @@
       <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -880,85 +1087,85 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -977,13 +1184,13 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="3" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -997,85 +1204,85 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1094,13 +1301,13 @@
       <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="3" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1114,85 +1321,85 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1211,13 +1418,13 @@
       <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="3" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1231,85 +1438,85 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1328,13 +1535,13 @@
       <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="3" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1348,85 +1555,85 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1445,13 +1652,13 @@
       <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="3" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1465,85 +1672,85 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1562,7 +1769,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -1570,7 +1777,7 @@
     <col min="4" max="4" width="112.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1584,7 +1791,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
@@ -1598,79 +1805,79 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="6"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>

</xml_diff>